<commit_message>
Correccion algunas tablas y datos
</commit_message>
<xml_diff>
--- a/db/Dia_materia_orquestal.xlsx
+++ b/db/Dia_materia_orquestal.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\Posgrado\Proyecto Titulacion\db\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Debian\home\andrew\Documents\Proyecto_Titulacion\Timetabling\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC21DDC-DC72-4C14-9F43-131C45E200AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B89EFEE9-409C-491B-A558-C9DE44CAD196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F0F29C3E-BF4A-4AD7-BD10-6518BCE807DD}"/>
+    <workbookView xWindow="7680" yWindow="3024" windowWidth="17280" windowHeight="8880" xr2:uid="{F0F29C3E-BF4A-4AD7-BD10-6518BCE807DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,15 +34,57 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>dia_semana</t>
-  </si>
-  <si>
-    <t>Viernes</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="17">
   <si>
     <t>id_materia</t>
+  </si>
+  <si>
+    <t>Martes</t>
+  </si>
+  <si>
+    <t>Jueves</t>
+  </si>
+  <si>
+    <t>INC-OC</t>
+  </si>
+  <si>
+    <t>INC-OG</t>
+  </si>
+  <si>
+    <t>INC-FL</t>
+  </si>
+  <si>
+    <t>OCA</t>
+  </si>
+  <si>
+    <t>OGA</t>
+  </si>
+  <si>
+    <t>OVA</t>
+  </si>
+  <si>
+    <t>OPA</t>
+  </si>
+  <si>
+    <t>OCB</t>
+  </si>
+  <si>
+    <t>OGB</t>
+  </si>
+  <si>
+    <t>OVB</t>
+  </si>
+  <si>
+    <t>OPB</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>False</t>
   </si>
 </sst>
 </file>
@@ -78,7 +120,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -394,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FB7C0C2-41BB-4AA1-B87F-681C55960262}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -405,17 +448,147 @@
     <col min="1" max="1" width="18.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>15</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>